<commit_message>
now i have updated my main file and added new features
</commit_message>
<xml_diff>
--- a/stud_data/STEP 1.xlsx
+++ b/stud_data/STEP 1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,10 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>18-03-2025 Status</t>
+          <t>20-03-2025 Status</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>18-03-2025 Time</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>19-03-2025 Status</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>19-03-2025 Time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>20-03-2025 Status</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>20-03-2025 Time</t>
         </is>
@@ -490,7 +470,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -499,27 +479,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17:59:56</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>18:37:13</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>04:41:52</t>
+          <t>13:48:06</t>
         </is>
       </c>
     </row>
@@ -533,7 +493,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -542,27 +502,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>18:00:27</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>04:50:57</t>
+          <t>13:48:15</t>
         </is>
       </c>
     </row>
@@ -575,35 +515,13 @@
           <t>Kamran Gulam</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>
@@ -618,35 +536,13 @@
           <t>Umer Akmal</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>
@@ -661,35 +557,13 @@
           <t>Abuzar hassan</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>18:36:47</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>

</xml_diff>